<commit_message>
sheet into two dim obj array
</commit_message>
<xml_diff>
--- a/testdata/orange_testdata.xlsx
+++ b/testdata/orange_testdata.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
-    <sheet name="validCredentialTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -374,9 +373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -431,16 +428,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
excel to two dim array dynamic
</commit_message>
<xml_diff>
--- a/testdata/orange_testdata.xlsx
+++ b/testdata/orange_testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>Password</t>
   </si>
@@ -54,6 +54,30 @@
   </si>
   <si>
     <t>peter123</t>
+  </si>
+  <si>
+    <t>peter124</t>
+  </si>
+  <si>
+    <t>peter125</t>
+  </si>
+  <si>
+    <t>peter126</t>
+  </si>
+  <si>
+    <t>peter127</t>
+  </si>
+  <si>
+    <t>peter128</t>
+  </si>
+  <si>
+    <t>peter129</t>
+  </si>
+  <si>
+    <t>peter130</t>
+  </si>
+  <si>
+    <t>peter131</t>
   </si>
 </sst>
 </file>
@@ -371,9 +395,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -425,6 +451,94 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel and dataprovider to invalid
</commit_message>
<xml_diff>
--- a/testdata/orange_testdata.xlsx
+++ b/testdata/orange_testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Password</t>
   </si>
@@ -50,34 +50,10 @@
     <t>dina123</t>
   </si>
   <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>peter123</t>
-  </si>
-  <si>
-    <t>peter124</t>
-  </si>
-  <si>
-    <t>peter125</t>
-  </si>
-  <si>
-    <t>peter126</t>
-  </si>
-  <si>
-    <t>peter127</t>
-  </si>
-  <si>
-    <t>peter128</t>
-  </si>
-  <si>
-    <t>peter129</t>
-  </si>
-  <si>
-    <t>peter130</t>
-  </si>
-  <si>
-    <t>peter131</t>
+    <t>Bala</t>
+  </si>
+  <si>
+    <t>bala123</t>
   </si>
 </sst>
 </file>
@@ -395,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,10 +396,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -442,100 +418,12 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commondataprovider for connecting excel
</commit_message>
<xml_diff>
--- a/testdata/orange_testdata.xlsx
+++ b/testdata/orange_testdata.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="validCredentialTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Password</t>
   </si>
@@ -54,16 +55,36 @@
   </si>
   <si>
     <t>bala123</t>
+  </si>
+  <si>
+    <t>Expected Url</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/index.php/dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,13 +107,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,7 +397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -430,4 +454,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>